<commit_message>
remove AHC examples from US Core
</commit_message>
<xml_diff>
--- a/input/images-source/dstu2-r4-table.xlsx
+++ b/input/images-source/dstu2-r4-table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/images-source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624D0277-BE94-544D-9552-5E867BB4973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33DE30A-5F21-A946-9AB6-B0C3732DDFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19620" yWindow="500" windowWidth="34120" windowHeight="28300" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
+    <workbookView xWindow="-34400" yWindow="-18220" windowWidth="34400" windowHeight="28300" xr2:uid="{9AFB64A6-2FE7-CB43-8C5B-B64EFE3BA62D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="110">
   <si>
     <t>DSTU2 Profile</t>
   </si>
@@ -321,12 +321,6 @@
     <t>US Core Jurisdiction Extension</t>
   </si>
   <si>
-    <t>US Core Sex For Clinical Use</t>
-  </si>
-  <si>
-    <t>Retired in version 6.0.0</t>
-  </si>
-  <si>
     <t>Version Retired</t>
   </si>
   <si>
@@ -361,19 +355,32 @@
   </si>
   <si>
     <t>In Version 6.0.0 derived from US Core Observation Clinical Test Result Profile</t>
+  </si>
+  <si>
+    <t>US Core USCDI Requirements Extension</t>
+  </si>
+  <si>
+    <t>This extension is only used on US Core Profile StructureDefinition elements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -396,12 +403,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,7 +727,7 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,7 +749,7 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -927,7 +935,7 @@
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1247,7 +1255,7 @@
         <v>86</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1264,7 +1272,7 @@
         <v>86</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1281,7 +1289,7 @@
         <v>86</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1298,7 +1306,7 @@
         <v>86</v>
       </c>
       <c r="E44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1306,7 +1314,7 @@
         <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
         <v>49</v>
@@ -1315,7 +1323,7 @@
         <v>86</v>
       </c>
       <c r="E45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1328,12 +1336,6 @@
       <c r="C46" t="s">
         <v>49</v>
       </c>
-      <c r="D46" t="s">
-        <v>86</v>
-      </c>
-      <c r="E46" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
@@ -1406,13 +1408,13 @@
         <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C53" t="s">
         <v>86</v>
       </c>
       <c r="E53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1420,13 +1422,13 @@
         <v>84</v>
       </c>
       <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" t="s">
         <v>101</v>
-      </c>
-      <c r="C54" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1445,13 +1447,13 @@
         <v>84</v>
       </c>
       <c r="B56" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" t="s">
         <v>100</v>
-      </c>
-      <c r="C56" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1524,12 +1526,6 @@
       <c r="C63" t="s">
         <v>49</v>
       </c>
-      <c r="D63" t="s">
-        <v>86</v>
-      </c>
-      <c r="E63" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -1547,18 +1543,18 @@
         <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C65" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C66" t="s">
         <v>86</v>
@@ -1569,10 +1565,13 @@
         <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>